<commit_message>
Update to herarchy and dataset
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/jojimenezt_unal_edu_co/Documents/Documentos/UNAL/NLP/project-NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="446" documentId="11_B72079981C130BA42D210E850FD72AC7B5CDEA4B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70C3E103-FABE-47D6-86DB-CA6DC77400CA}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="11_B72079981C130BA42D210E850FD72AC7B5CDEA4B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55C9EE02-8886-4418-9234-51850E68A3E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2606,7 +2606,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K123" sqref="K122:K123"/>
+      <selection pane="bottomLeft" activeCell="L122" sqref="L122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>